<commit_message>
Add Allemagne, pologne UI test
</commit_message>
<xml_diff>
--- a/src/excelExportAndFileIO/jeu_de_test_PL.xlsx
+++ b/src/excelExportAndFileIO/jeu_de_test_PL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -653,7 +653,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>